<commit_message>
Certificate Master UI corrected.
</commit_message>
<xml_diff>
--- a/Insurance/insurance_templates/mcc_template.xlsx
+++ b/Insurance/insurance_templates/mcc_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr dateCompatibility="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\algaeh-monorepo\Insurance\insurance_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Project/algaeh-monorepo/Insurance/insurance_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5D84A9A8-180E-4A3E-AF4A-86D8DD1FE7E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D6C8085F-4107-6A49-B7E0-C7690A49298B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -231,6 +231,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -239,18 +251,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -345,22 +345,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>190501</xdr:colOff>
+      <xdr:colOff>12700</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1105064</xdr:colOff>
+      <xdr:colOff>860994</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1162050</xdr:rowOff>
+      <xdr:rowOff>1193801</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Logo.png">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{244BBDAD-5274-4221-803F-08072733602E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1C65354-AF2F-724D-A75E-81A4427476D6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -369,49 +369,19 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="190501" y="123826"/>
-          <a:ext cx="2248063" cy="1038224"/>
+          <a:off x="12700" y="1"/>
+          <a:ext cx="2372294" cy="1193800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800%"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -744,39 +714,39 @@
   <dimension ref="A1:N413"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="31" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="39" style="6" customWidth="1"/>
-    <col min="9" max="14" width="16.28515625" style="7" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="8"/>
+    <col min="9" max="14" width="16.33203125" style="7" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="11" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+    <row r="1" spans="1:14" s="15" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="2" spans="1:14" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12" t="s">
+      <c r="E2" s="16"/>
+      <c r="F2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
@@ -784,21 +754,21 @@
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
     </row>
-    <row r="3" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13" t="s">
+      <c r="E3" s="17"/>
+      <c r="F3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -806,33 +776,33 @@
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="16" t="s">
+    <row r="4" spans="1:14" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16" t="s">
+      <c r="L4" s="13"/>
+      <c r="M4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="N4" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -876,414 +846,414 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="137" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="138" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="150" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="164" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="165" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="167" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="168" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="169" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="170" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="171" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="172" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="173" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="174" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="175" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="176" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="177" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="178" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="179" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="180" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="181" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="182" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="183" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="184" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="185" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="186" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="187" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="188" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="189" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="190" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="191" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="192" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="193" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="194" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="195" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="196" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="197" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="198" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="199" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="200" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="201" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="202" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="203" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="204" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="205" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="206" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="207" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="208" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="209" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="210" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="211" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="213" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="215" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="217" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="218" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="219" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="220" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="221" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="222" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="223" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="224" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="225" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="229" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="232" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="233" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="264" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="265" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="268" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="273" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="275" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="276" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="277" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="278" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="281" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="293" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="296" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="299" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="307" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="331" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="334" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="336" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="337" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="338" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="340" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="358" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="360" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="367" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="380" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="381" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="383" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="385" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="386" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="392" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="7" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="8" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="9" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="17" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="18" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="20" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="21" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="22" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="23" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="24" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="26" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="28" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="29" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="32" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="33" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="35" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="36" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="37" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="38" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="39" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="40" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="41" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="42" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="43" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="44" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="45" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="46" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="47" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="48" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="49" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="50" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="51" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="52" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="53" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="54" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="55" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="56" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="57" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="58" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="59" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="60" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="61" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="62" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="63" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="64" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="65" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="66" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="67" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="68" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="69" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="70" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="71" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="72" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="73" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="74" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="75" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="76" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="77" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="78" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="79" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="80" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="81" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="82" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="83" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="84" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="85" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="86" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="87" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="88" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="89" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="90" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="91" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="92" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="93" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="94" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="95" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="96" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="97" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="98" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="99" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="100" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="101" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="102" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="103" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="104" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="105" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="106" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="107" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="108" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="109" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="110" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="111" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="113" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="114" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="115" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="116" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="117" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="118" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="119" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="120" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="121" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="122" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="123" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="124" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="125" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="126" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="127" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="128" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="129" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="130" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="131" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="132" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="133" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="134" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="135" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="136" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="137" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="138" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="139" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="140" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="141" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="142" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="143" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="144" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="145" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="146" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="147" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="148" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="149" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="150" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="151" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="152" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="153" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="154" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="155" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="156" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="157" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="158" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="159" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="160" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="161" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="162" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="163" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="164" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="165" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="166" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="167" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="168" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="169" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="170" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="171" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="172" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="173" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="174" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="175" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="176" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="177" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="178" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="179" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="180" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="181" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="182" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="183" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="184" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="185" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="186" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="187" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="188" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="189" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="190" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="191" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="192" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="193" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="194" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="195" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="196" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="197" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="198" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="199" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="200" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="201" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="202" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="203" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="204" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="205" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="206" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="207" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="208" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="209" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="210" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="211" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="212" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="213" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="214" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="215" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="216" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="217" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="218" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="219" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="220" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="221" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="222" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="223" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="224" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="225" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="226" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="227" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="228" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="229" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="230" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="231" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="232" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="233" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="234" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="235" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="236" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="237" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="238" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="239" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="240" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="241" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="242" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="243" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="244" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="245" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="246" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="247" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="248" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="249" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="250" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="251" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="252" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="253" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="254" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="255" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="256" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="257" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="258" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="259" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="260" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="261" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="262" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="263" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="264" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="265" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="266" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="267" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="268" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="269" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="270" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="271" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="272" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="273" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="274" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="275" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="276" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="277" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="278" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="279" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="280" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="281" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="282" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="283" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="284" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="285" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="286" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="287" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="288" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="289" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="290" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="291" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="292" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="293" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="294" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="295" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="296" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="297" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="298" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="299" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="300" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="301" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="302" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="303" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="304" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="305" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="306" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="307" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="308" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="309" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="310" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="311" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="312" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="313" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="314" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="315" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="316" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="317" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="318" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="319" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="320" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="321" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="322" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="323" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="324" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="325" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="326" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="327" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="328" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="329" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="330" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="331" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="332" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="333" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="334" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="335" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="336" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="337" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="338" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="339" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="340" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="341" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="342" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="343" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="344" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="345" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="346" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="347" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="348" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="349" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="350" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="351" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="352" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="353" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="354" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="355" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="356" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="357" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="358" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="359" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="360" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="361" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="362" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="363" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="364" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="365" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="366" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="367" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="368" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="369" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="370" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="371" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="372" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="373" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="374" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="375" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="376" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="377" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="378" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="379" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="380" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="381" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="382" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="383" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="384" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="385" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="386" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="387" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="388" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="389" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="390" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="391" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="392" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="393" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="394" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="395" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="396" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="397" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="398" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="399" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="400" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="401" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="402" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="403" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="404" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="405" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="406" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="407" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="408" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="409" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="410" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="411" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="412" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="413" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:XFD1"/>

</xml_diff>

<commit_message>
mcc template few changes
</commit_message>
<xml_diff>
--- a/Insurance/insurance_templates/mcc_template.xlsx
+++ b/Insurance/insurance_templates/mcc_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr dateCompatibility="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Project/algaeh-monorepo/Insurance/insurance_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D6C8085F-4107-6A49-B7E0-C7690A49298B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1381B823-DCBA-334A-812D-3A9E98A57342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="25" uniqueCount="25">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="29" uniqueCount="27">
   <si>
     <t>Patient Name</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>Patient Payable</t>
+  </si>
+  <si>
+    <t>COMPANY ADDRESS:-</t>
+  </si>
+  <si>
+    <t>STATEMENT NO.:-</t>
   </si>
 </sst>
 </file>
@@ -172,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <start/>
       <end/>
@@ -195,11 +201,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <start style="thin">
+        <color indexed="64"/>
+      </start>
+      <end/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -243,14 +286,23 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -351,7 +403,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>860994</xdr:colOff>
+      <xdr:colOff>1089594</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1193801</xdr:rowOff>
     </xdr:to>
@@ -714,66 +766,91 @@
   <dimension ref="A1:N413"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F3" sqref="F3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="31" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39" style="6" customWidth="1"/>
-    <col min="9" max="14" width="16.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="7" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5" style="7" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="15" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1" spans="1:14" s="17" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D1" s="18"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="20"/>
+    </row>
     <row r="2" spans="1:14" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16" t="s">
+      <c r="J2" s="15"/>
+      <c r="K2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17" t="s">
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
@@ -1255,14 +1332,18 @@
     <row r="412" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="413" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A1:XFD1"/>
+  <mergeCells count="11">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="F3:H3"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:M3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions gridLines="1"/>

</xml_diff>

<commit_message>
MCC Insurance Statement changes
</commit_message>
<xml_diff>
--- a/Insurance/insurance_templates/mcc_template.xlsx
+++ b/Insurance/insurance_templates/mcc_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Project/algaeh-monorepo/Insurance/insurance_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1381B823-DCBA-334A-812D-3A9E98A57342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3B80ABA8-587D-4A4D-8479-FB322A1AAD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="29" uniqueCount="27">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="26" uniqueCount="26">
   <si>
     <t>Patient Name</t>
   </si>
@@ -71,18 +71,9 @@
     <t>MEDICAL CLAIMS STATEMENT FOR THE MONTH OF :-</t>
   </si>
   <si>
-    <t>NAME OF HOSPITAL:-</t>
-  </si>
-  <si>
-    <t>#CLINICNAME</t>
-  </si>
-  <si>
     <t>NAME OF COMPANY:-</t>
   </si>
   <si>
-    <t>#COMPANYNAME</t>
-  </si>
-  <si>
     <t>#FDATE - #TDATE</t>
   </si>
   <si>
@@ -110,10 +101,30 @@
     <t>Patient Payable</t>
   </si>
   <si>
-    <t>COMPANY ADDRESS:-</t>
-  </si>
-  <si>
     <t>STATEMENT NO.:-</t>
+  </si>
+  <si>
+    <t>#STATEMENTNO</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   Modern Care Medical Complex   
+  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Azizia, 16 B St, Al Jisr, Al Khobar 34714, 
+   Kingdom of Saudi Arabia
+   Tel: 929927221
+   VAT: 310497403200003</t>
+    </r>
+  </si>
+  <si>
+    <t>#COMPANYNAME - #INSADDRESS</t>
   </si>
 </sst>
 </file>
@@ -242,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -253,56 +264,65 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -397,22 +417,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1089594</xdr:colOff>
+      <xdr:colOff>1076894</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1193801</xdr:rowOff>
+      <xdr:rowOff>1193800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1C65354-AF2F-724D-A75E-81A4427476D6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7ED7C715-4BB4-D045-ADC4-71BA8433EA93}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -428,7 +448,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12700" y="1"/>
+          <a:off x="0" y="0"/>
           <a:ext cx="2372294" cy="1193800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -766,120 +786,118 @@
   <dimension ref="A1:N413"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:H3"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="8"/>
+    <col min="6" max="6" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27" style="7" customWidth="1"/>
+    <col min="16" max="16384" width="8.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="17" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
+    <row r="1" spans="1:14" s="13" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
       <c r="N1" s="20"/>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15" t="s">
+    <row r="2" spans="1:14" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="18"/>
+      <c r="M2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="9"/>
+      <c r="N2" s="18"/>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16" t="s">
+      <c r="A3" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="23"/>
+      <c r="M3" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16" t="s">
+      <c r="N3" s="20"/>
+    </row>
+    <row r="4" spans="1:14" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="4"/>
+      <c r="J4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -890,7 +908,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
@@ -899,7 +917,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>6</v>
@@ -908,7 +926,7 @@
         <v>2</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>8</v>
@@ -1332,18 +1350,15 @@
     <row r="412" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="413" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:H3"/>
+  <mergeCells count="8">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
     <mergeCell ref="D1:N1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions gridLines="1"/>

</xml_diff>